<commit_message>
Removed unnecesery .xlsx file maker
</commit_message>
<xml_diff>
--- a/Styled_Results.xlsx
+++ b/Styled_Results.xlsx
@@ -462,7 +462,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Logistics Analyst</t>
         </is>
       </c>
     </row>
@@ -539,35 +539,35 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Local Truck Driver - 1yr EXP Required - Dry Van - CPC Logistics</t>
+          <t>Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Logistics Technology Solutions Specialist</t>
+          <t>Local Truck Driver - 1yr EXP Required - Dry Van - CPC Logistics</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Logistics Manager</t>
+          <t>Logistics Technology Solutions Specialist</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Logistics Specialist</t>
+          <t>Logistics Manager</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated nighttime truck driver</t>
+          <t>Logistics Specialist</t>
         </is>
       </c>
     </row>
@@ -609,28 +609,28 @@
     <row r="23">
       <c r="A23" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver Company - 1yr EXP Required - Local - Dry Van - CPC Logistics</t>
+          <t>Midwest Logistics Systems Dedicated nighttime truck driver</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Company Driver - 1yr EXP Required - Local - Dry Van - CPC Logistics</t>
+          <t>Truck Driver Company - 1yr EXP Required - Local - Dry Van - CPC Logistics</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="inlineStr">
         <is>
-          <t>Class A CDL Company Driver - 1yr EXP Required - Local - Dry Van - CPC Logistics</t>
+          <t>CDL-A Company Driver - 1yr EXP Required - Local - Dry Van - CPC Logistics</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Part-time Dedicated truck driver</t>
+          <t>Class A CDL Company Driver - 1yr EXP Required - Local - Dry Van - CPC Logistics</t>
         </is>
       </c>
     </row>
@@ -658,49 +658,49 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>Purchasing, Supply and Logistics</t>
+          <t>Midwest Logistics Systems Part-time Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="inlineStr">
         <is>
-          <t>Regional Truck Driver Company - 1yr EXP Required - Dry Van - $2k per week - Transervice Logistics</t>
+          <t>Purchasing, Supply and Logistics</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Company Driver - 1yr EXP Required - Regional - Dry Van - $2k per week - Transervice Logistics</t>
+          <t>Regional Truck Driver Company - 1yr EXP Required - Dry Van - $2k per week - Transervice Logistics</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Company Driver - 1yr EXP Required - OTR - Tanker - N Endorsements Required - Talon Logistics</t>
+          <t>CDL-A Company Driver - 1yr EXP Required - Regional - Dry Van - $2k per week - Transervice Logistics</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Part-time Dedicated truck driver - weekends</t>
+          <t>CDL-A Company Driver - 1yr EXP Required - OTR - Tanker - N Endorsements Required - Talon Logistics</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Midwest Logistics Systems Part-time Dedicated truck driver - weekends</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>Logistics Specialist</t>
+          <t>Logistics</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator</t>
+          <t>Logistics Specialist</t>
         </is>
       </c>
     </row>
@@ -742,1120 +742,1120 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Team Driver - 1yr EXP Required - Regional - Dry Van - Transervice Logistics</t>
+          <t>Logistics Coordinator</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="inlineStr">
         <is>
-          <t>LOGISTICS COORDINATOR</t>
+          <t>CDL-A Team Driver - 1yr EXP Required - Regional - Dry Van - Transervice Logistics</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator</t>
+          <t>LOGISTICS COORDINATOR</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Logistics Support Specialist</t>
+          <t>Associate Business Systems Analyst</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>LOGISTICS PRICING ANALYST</t>
+          <t>Supply Chain Financial Analyst</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Project Logistics Leader</t>
+          <t>Logistics Coordinator</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator II</t>
+          <t>Logistics Support Specialist</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="inlineStr">
         <is>
-          <t>Logistics Analyst</t>
+          <t>LOGISTICS PRICING ANALYST</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>Logistics &amp; Materials Manager</t>
+          <t>Ecomm Distribution Manager</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>Logistics Analyst</t>
+          <t>Project Logistics Leader</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>Logistics Associate</t>
+          <t>Logistics Coordinator II</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="inlineStr">
         <is>
-          <t>Regional Truck Driver Company - 1yr EXP Required - Dry Van - $90k per year - Transervice Logistics</t>
+          <t>Logistics &amp; Materials Manager</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Logistics Analyst</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="inlineStr">
         <is>
-          <t>Logistics Representative</t>
+          <t>Logistics Associate</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>Driver CDL - 1st Shift</t>
+          <t>Warehouse Operations Supervisor - 3rd Shift</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="inlineStr">
         <is>
-          <t>Logistics Engineer</t>
+          <t>Regional Truck Driver Company - 1yr EXP Required - Dry Van - $90k per year - Transervice Logistics</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>Logistics Analyst</t>
+          <t>Logistics</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="inlineStr">
         <is>
-          <t>Logistics Manager</t>
+          <t>Logistics Representative</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>Logistics Analyst, Senior</t>
+          <t>Driver CDL - 1st Shift</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>Logistics Management Specialist</t>
+          <t>Manager, Procurement</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Senior Logistics Analyst</t>
+          <t>Logistics Engineer</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator-10 Hour Shift</t>
+          <t>Logistics Analyst</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>Director, Logistics</t>
+          <t>Logistics Manager</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>Associate Director - Digital Logistics, Global Logistics</t>
+          <t>Logistics Analyst, Senior</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>Sr. Associate - Digital Logistics, Global Logistics</t>
+          <t>Logistics Management Specialist</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="3" t="inlineStr">
         <is>
-          <t>Principal Logistics Specialist - EDI Analyst</t>
+          <t>Senior Logistics Analyst</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>Logistics Manager</t>
+          <t>Logistics Coordinator-10 Hour Shift</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="3" t="inlineStr">
         <is>
-          <t>Controller - Logistics</t>
+          <t>Director, Logistics</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>Trading Operations Team Lead</t>
+          <t>FPA Manager - Hybrid, Hanahan, SC</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="3" t="inlineStr">
         <is>
-          <t>Logistics Supervisor</t>
+          <t>Associate Director - Digital Logistics, Global Logistics</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>Logistics Support Specialist</t>
+          <t>Sr. Associate - Digital Logistics, Global Logistics</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Principal Logistics Specialist - EDI Analyst</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>Warehouse Logistics</t>
+          <t>Logistics Manager</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="3" t="inlineStr">
         <is>
-          <t>Driver CDL - 3rd shift</t>
+          <t>Controller - Logistics</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>Logistics Engineer IV</t>
+          <t>Logistics Supervisor</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="3" t="inlineStr">
         <is>
-          <t>Logistics Engineer IV</t>
+          <t>Trading Operations Team Lead</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>Logistics Engineer IV</t>
+          <t>Logistics Support Specialist</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="3" t="inlineStr">
         <is>
-          <t>Logistics Analyst</t>
+          <t>Logistics</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator</t>
+          <t>Warehouse Logistics</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator</t>
+          <t>Logistics Engineer IV</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator</t>
+          <t>Logistics Engineer IV</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="3" t="inlineStr">
         <is>
-          <t>Controller - Logistics</t>
+          <t>Logistics Engineer IV</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>Mechatronic Maintenance Technician II - 2nd Shift</t>
+          <t>Driver CDL - 3rd shift</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Principal Logistics Engineer</t>
+          <t>Logistics Analyst</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Logistics Account Business &amp; Development Manager</t>
+          <t>Logistics Coordinator</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="3" t="inlineStr">
         <is>
-          <t>Logistics Technician</t>
+          <t>Logistics Coordinator</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>Sourcing and Logistics Specialist</t>
+          <t>Logistics Coordinator</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="3" t="inlineStr">
         <is>
-          <t>Senior Manager Logistics</t>
+          <t>Controller - Logistics</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>Logistics Support Specialist</t>
+          <t>Principal Logistics Engineer</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="3" t="inlineStr">
         <is>
-          <t>Logistics and Shelter Liaison (Hiring Immediately)</t>
+          <t>Mechatronic Maintenance Technician II - 2nd Shift</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>Animal Logistics Specialist (Hiring Immediately)</t>
+          <t>Manager, Corporate Communications</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="3" t="inlineStr">
         <is>
-          <t>Sr. Logistics Admin</t>
+          <t>Logistics Account Business &amp; Development Manager</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Company Driver - 2yrs EXP Required - Dedicated - Dry Van - $85k per year - Logos Logistics</t>
+          <t>Logistics Technician</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="3" t="inlineStr">
         <is>
-          <t>Senior Logistics Analyst</t>
+          <t>Sourcing and Logistics Specialist</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>Logistics Claims Specialist</t>
+          <t>Senior Manager Logistics</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="3" t="inlineStr">
         <is>
-          <t>Accounting Manager (Logistics)</t>
+          <t>Senior Manager, Procurement</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>(Agile1)Logistical Planner, Senior</t>
+          <t>Logistics Support Specialist</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="3" t="inlineStr">
         <is>
-          <t>Logistics Supervisor - 1st Shift</t>
+          <t>Conference Services Manager</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>Logistics Support Specialist</t>
+          <t>Residential Sales</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3" t="inlineStr">
         <is>
-          <t>Logistics Hauler BW</t>
+          <t>Logistics and Shelter Liaison (Hiring Immediately)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>Security Guard - Logistics Company</t>
+          <t>Animal Logistics Specialist (Hiring Immediately)</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="3" t="inlineStr">
         <is>
-          <t>Logistics Accounts Payable Clerk</t>
+          <t>Sr. Logistics Admin</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>Logistics Accounts Payable Clerk</t>
+          <t>CDL-A Company Driver - 2yrs EXP Required - Dedicated - Dry Van - $85k per year - Logos Logistics</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="3" t="inlineStr">
         <is>
-          <t>Logistics Sales Director</t>
+          <t>Senior Logistics Analyst</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>Logistics Sales Representative</t>
+          <t>Training Coordinator (9617)</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="3" t="inlineStr">
         <is>
-          <t>Logistics Sales Representative</t>
+          <t>Material Handler, Second Shift</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>Accounting Manager (Logistics)</t>
+          <t>Logistics Claims Specialist</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="3" t="inlineStr">
         <is>
-          <t>Warehouse and Logistics - Inventory Specialist</t>
+          <t>Accounting Manager (Logistics)</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>Pharmacy Logistics Technician</t>
+          <t>(Agile1)Logistical Planner, Senior</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="3" t="inlineStr">
         <is>
-          <t>Specialist, Domestic Logistics and Distribution</t>
+          <t>Logistics Supervisor - 1st Shift</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>Wendy's Assistant Manager</t>
+          <t>Logistics Support Specialist</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver Company - 1yr EXP Required - Local - Dry Van - $1.75k per week - CPC Logistics</t>
+          <t>Logistics Hauler BW</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Company Driver - 1yr EXP Required - Local - Dry Van - $1.75k per week - CPC Logistics</t>
+          <t>Security Guard - Logistics Company</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Logistics Accounts Payable Clerk</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>Engineer: (Coordinator, logistical operations, procedures)</t>
+          <t>Logistics Accounts Payable Clerk</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="3" t="inlineStr">
         <is>
-          <t>Logistics Protection Security &amp; Risk Manager</t>
+          <t>Logistics Sales Director</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>Sr. Logistics Manager - 1st Shift</t>
+          <t>Logistics Sales Representative</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="3" t="inlineStr">
         <is>
-          <t>Part-Time Warehouse Logistics</t>
+          <t>Logistics Sales Representative</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>Logistics Hauler Airport Warehouse</t>
+          <t>Accounting Manager (Logistics)</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3" t="inlineStr">
         <is>
-          <t>Part-Time Logistics Hauler</t>
+          <t>Warehouse and Logistics - Inventory Specialist</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>Plumber, Installer, Logistics Technician</t>
+          <t>Pharmacy Logistics Technician</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="3" t="inlineStr">
         <is>
-          <t>Air Logistics Warehouse Associate</t>
+          <t>Trader - Biodiesel</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>Trading Operations Manager</t>
+          <t>Wendy's Assistant Manager</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver Company - 2yrs EXP Required - Dedicated - Dry Van - $85k per year - Logos Logistics</t>
+          <t>Truck Driver Company - 1yr EXP Required - Local - Dry Van - $1.75k per week - CPC Logistics</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>Logistics Alternative Raw Materials Coordinator (Geocycle)</t>
+          <t>CDL-A Company Driver - 1yr EXP Required - Local - Dry Van - $1.75k per week - CPC Logistics</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="3" t="inlineStr">
         <is>
-          <t>Logistics Sales Development Intern</t>
+          <t>Logistics</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>Class A CDL Company Driver - 1yr EXP Required - Regional - Dry Van - $104k per year - Penske - 2502264 - Stanfield, OR</t>
+          <t>Engineer: (Coordinator, logistical operations, procedures)</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="3" t="inlineStr">
         <is>
-          <t>CDL-A Company Driver - 1yr EXP Required - Regional - Dry Van - $104k per year - Penske - 2502264 - Stanfield, OR</t>
+          <t>Logistics Protection Security &amp; Risk Manager</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>Regional Truck Driver Company - 1yr EXP Required - Dry Van - $104k per year - Penske - 2502264 - Stanfield, OR</t>
+          <t>Sr. Logistics Manager - 1st Shift</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="3" t="inlineStr">
         <is>
-          <t>Manager, Supply Chain Shipping and Logistics</t>
+          <t>Part-Time Warehouse Logistics</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>Logistics Maintenance Technician (Night Shift)</t>
+          <t>Logistics Hauler Airport Warehouse</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="3" t="inlineStr">
         <is>
-          <t>Logistics Supervisor - Night Shift</t>
+          <t>Part-Time Logistics Hauler</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>Logistics Supervisor - 3rd Shift</t>
+          <t>Plumber, Installer, Logistics Technician</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="3" t="inlineStr">
         <is>
-          <t>Logistics Supervisor - 3rd Shift</t>
+          <t>Air Logistics Warehouse Associate</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>Senior Logistics Analyst - Aviation Support</t>
+          <t>Truck Driver Company - 2yrs EXP Required - Dedicated - Dry Van - $85k per year - Logos Logistics</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="3" t="inlineStr">
         <is>
-          <t>Security Guard Logistics 2nd Shift</t>
+          <t>Logistics Alternative Raw Materials Coordinator (Geocycle)</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>Operations Logistics Support - Pleasant Prairie, WI</t>
+          <t>Trading Operations Manager</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="3" t="inlineStr">
         <is>
-          <t>Urgent! Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Logistics Sales Development Intern</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated nighttime truck driver</t>
+          <t>Local CDL A Driver NO TOUCH FREIGHT</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="3" t="inlineStr">
         <is>
-          <t>Security Guard Logistics Part Time Weekends</t>
+          <t>CDL A Truck Driver - Competitive Pay</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>Logistics Hauler Downtown (Full-Time)</t>
+          <t>Experienced CDL A Driver - No Touch Freight</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A -Penske Logistics</t>
+          <t>Experienced CDL Driver - Local</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - CDL Class A - Penske Logistics</t>
+          <t>CDL A Truck Driver - No Touch Freights</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A - Penske Logistics</t>
+          <t>Class A CDL Company Driver - 1yr EXP Required - Regional - Dry Van - $104k per year - Penske - 2502264 - Stanfield, OR</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>Endorsements Required - Transervice Logistics</t>
+          <t>CDL-A Company Driver - 1yr EXP Required - Regional - Dry Van - $104k per year - Penske - 2502264 - Stanfield, OR</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="3" t="inlineStr">
         <is>
-          <t>Quick Air Logistics Warehouse Specialist</t>
+          <t>Regional Truck Driver Company - 1yr EXP Required - Dry Van - $104k per year - Penske - 2502264 - Stanfield, OR</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>QuickSTAT Air Logistics Warehouse Specialist</t>
+          <t>Manager, Supply Chain Shipping and Logistics</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="3" t="inlineStr">
         <is>
-          <t>Field Admin</t>
+          <t>Logistics Maintenance Technician (Night Shift)</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="3" t="inlineStr">
         <is>
-          <t>KY Driver (Louisville)</t>
+          <t>Logistics Supervisor - Night Shift</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="3" t="inlineStr">
         <is>
-          <t>Group Director of Customer Logistics - Freight Brokerage</t>
+          <t>Logistics Supervisor - 3rd Shift</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>Senior Specialist - Logistics &amp; Global Trade Compliance</t>
+          <t>Logistics Supervisor - 3rd Shift</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="3" t="inlineStr">
         <is>
-          <t>Inventory Control Specialist I -Service &amp; Logistics</t>
+          <t>Senior Logistics Analyst - Aviation Support</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>Cash Processor- Warehouse</t>
+          <t>Clerk - 1st Shift</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="3" t="inlineStr">
         <is>
-          <t>Logistics Supervisor- 3rd/Swing Shift</t>
+          <t>Security Guard Logistics 2nd Shift</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>RN Transplant Coordinator</t>
+          <t>Warehouse Order Selector | 2nd Shift</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="3" t="inlineStr">
         <is>
-          <t>Logistics/Logistics Specialist</t>
+          <t>Operations Logistics Support - Pleasant Prairie, WI</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Urgent! Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="3" t="inlineStr">
         <is>
-          <t>Superintendent I - Single Family</t>
+          <t>Midwest Logistics Systems Dedicated nighttime truck driver</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>Superintendent I - Multi Family</t>
+          <t>Security Guard Logistics Part Time Weekends</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A - Penske Logistics</t>
+          <t>Logistics Hauler Downtown (Full-Time)</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A - Penske Logistics</t>
+          <t>Truck Driver - Local Class A -Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated truck driver (Immediate Start)</t>
+          <t>Truck Driver - CDL Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>▷ Urgent Search! Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Truck Driver - Local Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="3" t="inlineStr">
         <is>
-          <t>[Immediate Start] Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Quick Air Logistics Warehouse Specialist</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>▷ (Immediate Start) Midwest Logistics Systems Dedicated truck driver</t>
+          <t>QuickSTAT Air Logistics Warehouse Specialist</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="3" t="inlineStr">
         <is>
-          <t>15h Left: Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Endorsements Required - Transervice Logistics</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>▷ [High Salary] Midwest Logistics Systems Dedicated truck driver</t>
+          <t>KY Driver (Louisville)</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="3" t="inlineStr">
         <is>
-          <t>▷ (15h Left) Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Class A CDL Driver</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>Immediate Start: Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Class A CDL Driver - At Home Nightly</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="3" t="inlineStr">
         <is>
-          <t>Assistant Transportation Manager</t>
+          <t>Industrial Maintenance Technician First Shift</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class B - Penske Logistics</t>
+          <t>Group Director of Customer Logistics - Freight Brokerage</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A - Penske Logistics</t>
+          <t>Senior Specialist - Logistics &amp; Global Trade Compliance</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A - Penske Logistics</t>
+          <t>Inventory Control Specialist I -Service &amp; Logistics</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="3" t="inlineStr">
         <is>
-          <t>Yard Truck Driver - Class A - Penske Logistics</t>
+          <t>Cash Processor- Warehouse</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - CDL Class A - Penske Logistics</t>
+          <t>Logistics Supervisor- 3rd/Swing Shift</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="3" t="inlineStr">
         <is>
-          <t>Truck Driver - Local Class A - Penske Logistics</t>
+          <t>RN Transplant Coordinator</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated truck driver</t>
+          <t>DC Facilities Manager</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Part Time Transfer Shuttle Driver</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>Lipsey Logistics - Weekday Night Tracking Associate</t>
+          <t>Catering Manager 4</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="3" t="inlineStr">
         <is>
-          <t>Event Logistics Support, 2025 PGA Championship</t>
+          <t>Logistics/Logistics Specialist</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>Forklift Operator (Logistics) - 8hr Days/Nights</t>
+          <t>Logistics</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="3" t="inlineStr">
         <is>
-          <t>EUD Technician/Site Lead</t>
+          <t>Superintendent I - Single Family</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Superintendent I - Multi Family</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>Truck Driver - Local Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Truck Driver - Local Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="3" t="inlineStr">
         <is>
-          <t>Intermodal Equipment Operator</t>
+          <t>Midwest Logistics Systems Dedicated truck driver (Immediate Start)</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>Logistics</t>
+          <t>▷ Urgent Search! Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Sr. Director, Quality Assurance – Materials Management &amp; Logistics</t>
+          <t>[Immediate Start] Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Logistics Manager - $5,000 Hiring Bonus</t>
+          <t>▷ (Immediate Start) Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="3" t="inlineStr">
         <is>
-          <t>Data Center Technician - I&amp;A Logistics Support 1</t>
+          <t>15h Left: Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Imperative Logistics - Logistics Coordinator</t>
+          <t>▷ [High Salary] Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="3" t="inlineStr">
         <is>
-          <t>Logistics Coordinator, Logistics Team</t>
+          <t>▷ (15h Left) Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>Logistic Clerk SCM. Logistics.</t>
+          <t>Immediate Start: Midwest Logistics Systems Dedicated truck driver</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="3" t="inlineStr">
         <is>
-          <t>Senior Manager, Procurement</t>
+          <t>Lead - 1st Shift</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>Data Center Technician - I&amp;A Logistics Support 2</t>
+          <t>Truck Driver - Local Class B - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="3" t="inlineStr">
         <is>
-          <t>▷ Only 24h Left! Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Truck Driver - Local Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>▷ (Apply in 3 Minutes) Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Truck Driver - Local Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="3" t="inlineStr">
         <is>
-          <t>Apply in 3 Minutes: Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Yard Truck Driver - Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>Midwest Logistics Systems Dedicated nighttime truck driver (Urgent Search)</t>
+          <t>Truck Driver - CDL Class A - Penske Logistics</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="3" t="inlineStr">
         <is>
-          <t>(3 Days Left) Midwest Logistics Systems Dedicated truck driver</t>
+          <t>Assistant Transportation Manager</t>
         </is>
       </c>
     </row>

</xml_diff>